<commit_message>
Se agrega CMS páginas Instructivos y Respuestos
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE6B30-F1A7-40BA-874B-197B7A9586C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46A8CB2-3E4D-4913-8D86-9EAF5CF3860A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D42B345-DB14-48C1-9A38-23908D3120ED}"/>
   </bookViews>
@@ -713,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -733,6 +733,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,44 +751,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="47">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -798,90 +774,49 @@
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -911,6 +846,53 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9"/>
@@ -948,6 +930,68 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -967,152 +1011,49 @@
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1123,10 +1064,61 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1225,14 +1217,14 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}" name="Tabla17" displayName="Tabla17" ref="H41:L44" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}" name="Tabla17" displayName="Tabla17" ref="H41:L44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="H41:L44" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C8F6ED57-5FD2-4FB3-A4A5-BC3965E98B15}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{65B99387-EDCD-429B-B81B-A4F58479A304}" name="IdProducto" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{5D9C0348-2DF4-47CC-977C-AAFB9F19E959}" name="Titulo" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{1CACB54F-DC9D-41AC-A04F-171EF34060DC}" name="URLImagen" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{824500A6-D872-42FD-9C38-60CB54869E2F}" name="Activo" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{C8F6ED57-5FD2-4FB3-A4A5-BC3965E98B15}" name="ID" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{65B99387-EDCD-429B-B81B-A4F58479A304}" name="IdProducto" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{5D9C0348-2DF4-47CC-977C-AAFB9F19E959}" name="Titulo" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{1CACB54F-DC9D-41AC-A04F-171EF34060DC}" name="URLImagen" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{824500A6-D872-42FD-9C38-60CB54869E2F}" name="Activo" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1260,8 +1252,8 @@
     <tableColumn id="3" xr3:uid="{650899D4-4E19-437F-9FCF-B4D26F2AA0DB}" name="Direccion"/>
     <tableColumn id="4" xr3:uid="{1E07E83B-09DC-40FD-907E-40F4CBC0A570}" name="IdProvincia"/>
     <tableColumn id="5" xr3:uid="{6138418F-A367-4A68-8F05-2638E82A22BC}" name="Telefono"/>
-    <tableColumn id="6" xr3:uid="{80260CDA-43B3-49C5-B2E8-6D4D4EE4367B}" name="Latitud" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{D1025C6A-57D3-4E57-916D-CF79774C6EAF}" name="Longitud" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{80260CDA-43B3-49C5-B2E8-6D4D4EE4367B}" name="Latitud" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{D1025C6A-57D3-4E57-916D-CF79774C6EAF}" name="Longitud" dataDxfId="33"/>
     <tableColumn id="8" xr3:uid="{FACFCBBE-C8C5-4011-911D-7F4D64577C47}" name="IdPagina"/>
     <tableColumn id="9" xr3:uid="{3EE8280A-E1AE-43CB-8AA3-681D1032743D}" name="Activo"/>
   </tableColumns>
@@ -1270,13 +1262,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6BCDECB-3201-4C98-AA8D-79812894A18B}" name="Tabla19" displayName="Tabla19" ref="K34:N37" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6BCDECB-3201-4C98-AA8D-79812894A18B}" name="Tabla19" displayName="Tabla19" ref="K34:N37" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="K34:N37" xr:uid="{36798AE9-B843-4477-9F23-32045BDEF7D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E050CEA3-2793-4698-9E45-C3447ADCD555}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{03295AE7-34B5-4134-9D2F-2268D15B310C}" name="IDProducto" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{1564E106-D50F-4573-A696-EE197325F0F3}" name="IDAtributo" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5F701778-C720-415C-9979-8380EB9AB80C}" name="Activo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E050CEA3-2793-4698-9E45-C3447ADCD555}" name="ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{03295AE7-34B5-4134-9D2F-2268D15B310C}" name="IDProducto" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{1564E106-D50F-4573-A696-EE197325F0F3}" name="IDAtributo" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{5F701778-C720-415C-9979-8380EB9AB80C}" name="Activo" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1289,8 +1281,8 @@
     <tableColumn id="1" xr3:uid="{76441B91-C9F3-418E-9F7A-2145EC66A51B}" name="ID"/>
     <tableColumn id="2" xr3:uid="{B7D7EADF-0604-4B90-A7CA-6537AE39152D}" name="Pronvincia"/>
     <tableColumn id="3" xr3:uid="{FBCCEEC7-DBEE-4480-8CBE-1F5805CA9202}" name="IdPais"/>
-    <tableColumn id="4" xr3:uid="{0A3D75EA-6C18-48E0-9489-C5D19B3AC70A}" name="Latitud" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{ACBD9873-D350-427F-993B-2B1B42296D9B}" name="Longitud" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{0A3D75EA-6C18-48E0-9489-C5D19B3AC70A}" name="Latitud" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{ACBD9873-D350-427F-993B-2B1B42296D9B}" name="Longitud" dataDxfId="25"/>
     <tableColumn id="6" xr3:uid="{957CA68C-6225-4C37-B8D5-8FF8C064FB1C}" name="Zoom"/>
     <tableColumn id="7" xr3:uid="{D19F9B22-3CC1-4E0E-B3DB-56D9B346F0CD}" name="Activo"/>
   </tableColumns>
@@ -1299,43 +1291,43 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D66B8F6B-A06F-42EB-B1CE-F5AC470DCC17}" name="Tabla20" displayName="Tabla20" ref="A62:D65" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D66B8F6B-A06F-42EB-B1CE-F5AC470DCC17}" name="Tabla20" displayName="Tabla20" ref="A62:D65" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A62:D65" xr:uid="{6995137C-E78D-4F26-A126-F3AEFE2A2B13}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7C1F763D-9A29-4F91-BB26-5F2CF68260F0}" name="ID" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{98E75056-4A9A-4C56-8FA5-EFD4D867777B}" name="Nombre" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{48A2AE2B-7A42-420C-8BB3-5F9F2AA01721}" name="Mail" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{7C1F763D-9A29-4F91-BB26-5F2CF68260F0}" name="ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{98E75056-4A9A-4C56-8FA5-EFD4D867777B}" name="Nombre" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{48A2AE2B-7A42-420C-8BB3-5F9F2AA01721}" name="Mail" dataDxfId="20">
       <calculatedColumnFormula>CONCATENATE(B63,"@andez.com.ar")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{31D99612-66DC-4B54-A747-6C39765D7B66}" name="Activo" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{31D99612-66DC-4B54-A747-6C39765D7B66}" name="Activo" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B2EAABA-4403-411A-98F0-A8284D43302C}" name="Tabla2021" displayName="Tabla2021" ref="F62:I65" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B2EAABA-4403-411A-98F0-A8284D43302C}" name="Tabla2021" displayName="Tabla2021" ref="F62:I65" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="F62:I65" xr:uid="{89087EED-CE2D-441A-9746-B0BA56EA9A63}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6D3F8F4E-2473-4BE6-A51E-C3C3E4C26133}" name="ID" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{12B007DF-889A-4CDB-93CC-EBEFCBD3A3E9}" name="Nombre" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{A94B5F86-8442-44DD-9C03-77F51D7F5B8D}" name="Telefono" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{6D3F8F4E-2473-4BE6-A51E-C3C3E4C26133}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{12B007DF-889A-4CDB-93CC-EBEFCBD3A3E9}" name="Nombre" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A94B5F86-8442-44DD-9C03-77F51D7F5B8D}" name="Telefono" dataDxfId="14">
       <calculatedColumnFormula>CONCATENATE(G63,"@andez.com.ar")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0E412ADD-9FF3-43E1-BDA1-A917D6B1E4D7}" name="Activo" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{0E412ADD-9FF3-43E1-BDA1-A917D6B1E4D7}" name="Activo" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{8F3FF2B6-156D-475C-B60E-2BBAE1F181CE}" name="Tabla21" displayName="Tabla21" ref="A69:D72" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{8F3FF2B6-156D-475C-B60E-2BBAE1F181CE}" name="Tabla21" displayName="Tabla21" ref="A69:D72" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A69:D72" xr:uid="{58000D4A-AEBA-4D49-B463-180C8FD8A937}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9F2D081-00F6-4B92-9DFE-6473CB6B3F38}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{DE65DD1F-F1BA-4548-A19A-4B9DD2857A6F}" name="Red" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{23F951D4-E519-45F7-81C5-69ED4EA385E4}" name="URLRed" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E5F1016C-C8F1-4FEA-B687-B57CB00F2E70}" name="Activo" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{E9F2D081-00F6-4B92-9DFE-6473CB6B3F38}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{DE65DD1F-F1BA-4548-A19A-4B9DD2857A6F}" name="Red" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{23F951D4-E519-45F7-81C5-69ED4EA385E4}" name="URLRed" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E5F1016C-C8F1-4FEA-B687-B57CB00F2E70}" name="Activo" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1355,13 +1347,13 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C769ADF8-2405-479D-8112-7564F0940768}" name="Tabla22" displayName="Tabla22" ref="F69:I72" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C769ADF8-2405-479D-8112-7564F0940768}" name="Tabla22" displayName="Tabla22" ref="F69:I72" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="F69:I72" xr:uid="{A2E83C68-75BA-4C98-B80E-E4E7E2B0B82C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{173EAAD2-F12F-4372-8FA2-00B32059C1EB}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{3E7AAA46-3847-4587-A43F-E688C1582045}" name="Titulo" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{7727AE8E-759C-4DE1-86AE-BDFED86835D0}" name="Descripcion" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2D33166C-2999-4BC9-8B00-7F06B4D84FF1}" name="Activo" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{173EAAD2-F12F-4372-8FA2-00B32059C1EB}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3E7AAA46-3847-4587-A43F-E688C1582045}" name="Titulo" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7727AE8E-759C-4DE1-86AE-BDFED86835D0}" name="Descripcion" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2D33166C-2999-4BC9-8B00-7F06B4D84FF1}" name="Activo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1786,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD350C1D-1850-4BF9-ABCF-FA1A23EC1542}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33:N33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1825,20 +1817,20 @@
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="I5" s="19" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="I5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1973,25 +1965,25 @@
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="G12" s="22" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="L12" s="22" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
+      <c r="L12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="24"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -2159,12 +2151,12 @@
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="F19" s="19" t="s">
         <v>109</v>
       </c>
@@ -2200,10 +2192,10 @@
       <c r="I20" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="27" t="s">
+      <c r="K20" t="s">
         <v>108</v>
       </c>
       <c r="L20" s="2" t="s">
@@ -2317,20 +2309,20 @@
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="I26" s="22" t="s">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="I26" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="24"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -2345,7 +2337,7 @@
       <c r="D27" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" t="s">
         <v>142</v>
       </c>
       <c r="F27" t="s">
@@ -2462,62 +2454,62 @@
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21"/>
-      <c r="K33" s="19" t="s">
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="24"/>
+      <c r="K33" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="21"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F34" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" t="s">
         <v>65</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" t="s">
         <v>116</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="L34" s="27" t="s">
+      <c r="K34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
         <v>114</v>
       </c>
-      <c r="M34" s="27" t="s">
+      <c r="M34" t="s">
         <v>115</v>
       </c>
-      <c r="N34" s="29" t="s">
+      <c r="N34" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2525,40 +2517,40 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="25">
-        <v>1</v>
-      </c>
-      <c r="C35" s="25">
-        <v>1</v>
-      </c>
-      <c r="D35" s="25" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="25">
-        <v>1</v>
-      </c>
-      <c r="F35" s="25">
-        <v>1</v>
-      </c>
-      <c r="G35" s="25" t="s">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="25" t="b">
+      <c r="H35" t="b">
         <v>1</v>
       </c>
       <c r="I35" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K35" s="28">
-        <v>1</v>
-      </c>
-      <c r="L35" s="27">
-        <v>1</v>
-      </c>
-      <c r="M35" s="27">
-        <v>1</v>
-      </c>
-      <c r="N35" s="29" t="b">
+      <c r="K35" s="1">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2566,40 +2558,40 @@
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="25">
-        <v>1</v>
-      </c>
-      <c r="C36" s="25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>2</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="25">
-        <v>1</v>
-      </c>
-      <c r="F36" s="25">
-        <v>1</v>
-      </c>
-      <c r="G36" s="25" t="s">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="25" t="b">
+      <c r="H36" t="b">
         <v>0</v>
       </c>
       <c r="I36" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K36" s="28">
+      <c r="K36" s="1">
         <v>2</v>
       </c>
-      <c r="L36" s="27">
-        <v>1</v>
-      </c>
-      <c r="M36" s="27">
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
         <v>2</v>
       </c>
-      <c r="N36" s="29" t="b">
+      <c r="N36" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2631,36 +2623,36 @@
       <c r="I37" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K37" s="30">
-        <v>3</v>
-      </c>
-      <c r="L37" s="31">
+      <c r="K37" s="3">
+        <v>3</v>
+      </c>
+      <c r="L37" s="4">
         <v>2</v>
       </c>
-      <c r="M37" s="31">
+      <c r="M37" s="4">
         <v>2</v>
       </c>
-      <c r="N37" s="32" t="b">
+      <c r="N37" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="H40" s="19" t="s">
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
+      <c r="H40" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="21"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="24"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -2681,19 +2673,19 @@
       <c r="F41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I41" s="27" t="s">
+      <c r="H41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
         <v>118</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J41" t="s">
         <v>119</v>
       </c>
-      <c r="K41" s="27" t="s">
+      <c r="K41" t="s">
         <v>120</v>
       </c>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2716,19 +2708,19 @@
       <c r="F42" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H42" s="28">
-        <v>1</v>
-      </c>
-      <c r="I42" s="27">
-        <v>1</v>
-      </c>
-      <c r="J42" s="27" t="s">
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
         <v>121</v>
       </c>
-      <c r="K42" s="27" t="s">
+      <c r="K42" t="s">
         <v>11</v>
       </c>
-      <c r="L42" s="29" t="b">
+      <c r="L42" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2751,19 +2743,19 @@
       <c r="F43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H43" s="28">
+      <c r="H43" s="1">
         <v>2</v>
       </c>
-      <c r="I43" s="27">
-        <v>1</v>
-      </c>
-      <c r="J43" s="27" t="s">
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
         <v>122</v>
       </c>
-      <c r="K43" s="27" t="s">
+      <c r="K43" t="s">
         <v>11</v>
       </c>
-      <c r="L43" s="29" t="b">
+      <c r="L43" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2786,39 +2778,39 @@
       <c r="F44" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H44" s="30">
-        <v>3</v>
-      </c>
-      <c r="I44" s="31">
+      <c r="H44" s="3">
+        <v>3</v>
+      </c>
+      <c r="I44" s="4">
         <v>2</v>
       </c>
-      <c r="J44" s="31" t="s">
+      <c r="J44" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K44" s="31" t="s">
+      <c r="K44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L44" s="32" t="b">
+      <c r="L44" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="21"/>
-      <c r="F47" s="19" t="s">
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+      <c r="F47" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="21"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="24"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -2962,17 +2954,17 @@
     </row>
     <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="21"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="24"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
@@ -3092,18 +3084,18 @@
     </row>
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="21"/>
-      <c r="F61" s="19" t="s">
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="F61" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="21"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="24"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
@@ -3214,18 +3206,18 @@
     </row>
     <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
-      <c r="F68" s="19" t="s">
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="24"/>
+      <c r="F68" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G68" s="20"/>
-      <c r="H68" s="20"/>
-      <c r="I68" s="21"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="24"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
@@ -3333,6 +3325,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F47:L47"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="I26:K26"/>
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A12:E12"/>
@@ -3340,19 +3345,6 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="G12:J12"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F47:L47"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrega CMS página Distribuidores. Modificaciones: se da estilo a las flechas de los select
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46A8CB2-3E4D-4913-8D86-9EAF5CF3860A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282749E7-1692-4B25-97CC-07510F2A1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D42B345-DB14-48C1-9A38-23908D3120ED}"/>
   </bookViews>
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD350C1D-1850-4BF9-ABCF-FA1A23EC1542}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:L19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2638,14 +2638,14 @@
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="24"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
       <c r="H40" s="22" t="s">
         <v>117</v>
       </c>
@@ -2796,21 +2796,21 @@
     </row>
     <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
-      <c r="F47" s="22" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="F47" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="21"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -2954,17 +2954,17 @@
     </row>
     <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="24"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="21"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
@@ -3325,6 +3325,8 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="I26:K26"/>
     <mergeCell ref="F68:I68"/>
     <mergeCell ref="F47:L47"/>
     <mergeCell ref="H40:L40"/>
@@ -3333,11 +3335,6 @@
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A54:I54"/>
     <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="I26:K26"/>
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A12:E12"/>
@@ -3345,6 +3342,9 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="K33:N33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrega CMS página Productos
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282749E7-1692-4B25-97CC-07510F2A1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D0FE2C-447B-46BF-B6FC-B0AF2492828A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D42B345-DB14-48C1-9A38-23908D3120ED}"/>
   </bookViews>
@@ -459,9 +459,6 @@
     <t>Jazz</t>
   </si>
   <si>
-    <t>AtributosPorProductos</t>
-  </si>
-  <si>
     <t>IDProducto</t>
   </si>
   <si>
@@ -547,6 +544,9 @@
   </si>
   <si>
     <t>FraseInstitucionalLinea</t>
+  </si>
+  <si>
+    <t>AtributosPorProductos (está en productos)</t>
   </si>
 </sst>
 </file>
@@ -1778,27 +1778,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD350C1D-1850-4BF9-ABCF-FA1A23EC1542}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
@@ -2338,7 +2337,7 @@
         <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" t="s">
         <v>35</v>
@@ -2454,23 +2453,23 @@
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
-      <c r="K33" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="24"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="21"/>
+      <c r="K33" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="21"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -2495,7 +2494,7 @@
         <v>65</v>
       </c>
       <c r="H34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>3</v>
@@ -2504,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="L34" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" t="s">
         <v>114</v>
-      </c>
-      <c r="M34" t="s">
-        <v>115</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>3</v>
@@ -2647,7 +2646,7 @@
       <c r="E40" s="20"/>
       <c r="F40" s="21"/>
       <c r="H40" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I40" s="23"/>
       <c r="J40" s="23"/>
@@ -2677,13 +2676,13 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" t="s">
         <v>118</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>119</v>
-      </c>
-      <c r="K41" t="s">
-        <v>120</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>3</v>
@@ -2715,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K42" t="s">
         <v>11</v>
@@ -2750,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K43" t="s">
         <v>11</v>
@@ -2785,7 +2784,7 @@
         <v>2</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>11</v>
@@ -3085,13 +3084,13 @@
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
       <c r="D61" s="24"/>
       <c r="F61" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G61" s="23"/>
       <c r="H61" s="23"/>
@@ -3128,7 +3127,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C63" s="10" t="str">
         <f>CONCATENATE(B63,"@andez.com.ar")</f>
@@ -3141,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H63" s="10">
         <v>45552646</v>
@@ -3155,7 +3154,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C64" s="10" t="str">
         <f t="shared" ref="C64:C65" si="0">CONCATENATE(B64,"@andez.com.ar")</f>
@@ -3168,7 +3167,7 @@
         <v>2</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H64" s="10">
         <v>45552646</v>
@@ -3182,7 +3181,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3195,7 +3194,7 @@
         <v>3</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H65" s="16">
         <v>1545552646</v>
@@ -3207,13 +3206,13 @@
     <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
       <c r="D68" s="24"/>
       <c r="F68" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G68" s="23"/>
       <c r="H68" s="23"/>
@@ -3224,11 +3223,11 @@
         <v>1</v>
       </c>
       <c r="B69" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="D69" s="18" t="s">
         <v>3</v>
       </c>
@@ -3236,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>57</v>
@@ -3250,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>11</v>
@@ -3262,7 +3261,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>58</v>
@@ -3276,7 +3275,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>11</v>
@@ -3288,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>58</v>
@@ -3302,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>11</v>
@@ -3314,7 +3313,7 @@
         <v>3</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H72" s="16" t="s">
         <v>58</v>
@@ -3325,6 +3324,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="K33:N33"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="F68:I68"/>
@@ -3335,16 +3344,6 @@
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A54:I54"/>
     <mergeCell ref="A40:F40"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="K33:N33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se modifica la Misión, Visión. Se agrega el Propósito y los Valores en el apartado Empresa. Se modifica tabla de planos en CMS Planos, se agrega hover a las imagenes de la tabla. Se agrega CMS página Configuración.
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D0FE2C-447B-46BF-B6FC-B0AF2492828A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004FE4DE-6D36-40CC-B083-C820EBD0BFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D42B345-DB14-48C1-9A38-23908D3120ED}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="153">
   <si>
     <t>Color</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Bidet Match baño calacata</t>
   </si>
   <si>
-    <t>InfoInstitucional_Mails</t>
-  </si>
-  <si>
     <t>Compras</t>
   </si>
   <si>
@@ -501,9 +498,6 @@
     <t>Ventas</t>
   </si>
   <si>
-    <t>InfoInstitucional_Telefonos</t>
-  </si>
-  <si>
     <t>Linea 1</t>
   </si>
   <si>
@@ -513,9 +507,6 @@
     <t>Celular</t>
   </si>
   <si>
-    <t>InfoInstitucional_Redes</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -531,22 +522,61 @@
     <t>Facebook</t>
   </si>
   <si>
-    <t>InfoInstitucional_Empresa</t>
-  </si>
-  <si>
-    <t>Historia</t>
-  </si>
-  <si>
-    <t>Mision</t>
-  </si>
-  <si>
-    <t>Vision</t>
-  </si>
-  <si>
     <t>FraseInstitucionalLinea</t>
   </si>
   <si>
     <t>AtributosPorProductos (está en productos)</t>
+  </si>
+  <si>
+    <t>Mails</t>
+  </si>
+  <si>
+    <t>Telefonos</t>
+  </si>
+  <si>
+    <t>RedesSociales</t>
+  </si>
+  <si>
+    <t>IdEmpresa</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Nombre S A</t>
+  </si>
+  <si>
+    <t>CUIT</t>
+  </si>
+  <si>
+    <t>20-55223344-1</t>
+  </si>
+  <si>
+    <t>Eva Peron 2543</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>Munro</t>
+  </si>
+  <si>
+    <t>Partido</t>
+  </si>
+  <si>
+    <t>Vicente Lopez</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>B1605BHA</t>
+  </si>
+  <si>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>Lun a Vier 8 a 16</t>
   </si>
 </sst>
 </file>
@@ -713,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -751,11 +781,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="56">
     <dxf>
       <font>
         <b val="0"/>
@@ -821,6 +852,38 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -862,7 +925,111 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9"/>
         </patternFill>
@@ -886,70 +1053,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9"/>
         </patternFill>
@@ -1174,7 +1277,7 @@
   <autoFilter ref="A13:E16" xr:uid="{D96833EF-4E6F-4FA0-A7A0-6E6817E2B38A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{317907DD-843B-4FA4-8837-A0A78A4A0507}" name="ID"/>
-    <tableColumn id="5" xr3:uid="{E0921BEC-D870-4C51-B3FC-23E013804DC3}" name="CodigoColor" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{E0921BEC-D870-4C51-B3FC-23E013804DC3}" name="CodigoColor" dataDxfId="55"/>
     <tableColumn id="2" xr3:uid="{8053C3DC-ACA4-4AAB-9AFB-34FBDDEBC52B}" name="NombreColor"/>
     <tableColumn id="4" xr3:uid="{1D3A10F0-E8C4-471A-B4A8-2001816AFFF2}" name="URLColor"/>
     <tableColumn id="3" xr3:uid="{D04813E9-6E48-439B-A711-735DEB41533C}" name="Activo"/>
@@ -1207,8 +1310,8 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C6605137-9E60-4417-BE9D-22DF41FEA57D}" name="ID"/>
     <tableColumn id="2" xr3:uid="{D82CDF84-BD14-4C63-ABBA-8F2236A9C0E4}" name="Pais"/>
-    <tableColumn id="3" xr3:uid="{FA78D055-E341-4362-A23A-0CCFC591E8FA}" name="Latitud" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{36EB177E-ACE1-4B78-A56A-A9F891312B25}" name="Longitud" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{FA78D055-E341-4362-A23A-0CCFC591E8FA}" name="Latitud" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{36EB177E-ACE1-4B78-A56A-A9F891312B25}" name="Longitud" dataDxfId="51"/>
     <tableColumn id="5" xr3:uid="{4122267C-292B-476B-8AB1-41CBE8A90AAF}" name="Zoom"/>
     <tableColumn id="7" xr3:uid="{0270C110-04E9-4179-AF06-958CA4E37E9B}" name="Activo"/>
   </tableColumns>
@@ -1217,14 +1320,14 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}" name="Tabla17" displayName="Tabla17" ref="H41:L44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}" name="Tabla17" displayName="Tabla17" ref="H41:L44" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="H41:L44" xr:uid="{EF32F6B3-AC45-462F-BE18-EFE2DD57FE9B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C8F6ED57-5FD2-4FB3-A4A5-BC3965E98B15}" name="ID" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{65B99387-EDCD-429B-B81B-A4F58479A304}" name="IdProducto" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{5D9C0348-2DF4-47CC-977C-AAFB9F19E959}" name="Titulo" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{1CACB54F-DC9D-41AC-A04F-171EF34060DC}" name="URLImagen" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{824500A6-D872-42FD-9C38-60CB54869E2F}" name="Activo" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{C8F6ED57-5FD2-4FB3-A4A5-BC3965E98B15}" name="ID" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{65B99387-EDCD-429B-B81B-A4F58479A304}" name="IdProducto" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{5D9C0348-2DF4-47CC-977C-AAFB9F19E959}" name="Titulo" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{1CACB54F-DC9D-41AC-A04F-171EF34060DC}" name="URLImagen" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{824500A6-D872-42FD-9C38-60CB54869E2F}" name="Activo" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1252,8 +1355,8 @@
     <tableColumn id="3" xr3:uid="{650899D4-4E19-437F-9FCF-B4D26F2AA0DB}" name="Direccion"/>
     <tableColumn id="4" xr3:uid="{1E07E83B-09DC-40FD-907E-40F4CBC0A570}" name="IdProvincia"/>
     <tableColumn id="5" xr3:uid="{6138418F-A367-4A68-8F05-2638E82A22BC}" name="Telefono"/>
-    <tableColumn id="6" xr3:uid="{80260CDA-43B3-49C5-B2E8-6D4D4EE4367B}" name="Latitud" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{D1025C6A-57D3-4E57-916D-CF79774C6EAF}" name="Longitud" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{80260CDA-43B3-49C5-B2E8-6D4D4EE4367B}" name="Latitud" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{D1025C6A-57D3-4E57-916D-CF79774C6EAF}" name="Longitud" dataDxfId="42"/>
     <tableColumn id="8" xr3:uid="{FACFCBBE-C8C5-4011-911D-7F4D64577C47}" name="IdPagina"/>
     <tableColumn id="9" xr3:uid="{3EE8280A-E1AE-43CB-8AA3-681D1032743D}" name="Activo"/>
   </tableColumns>
@@ -1262,13 +1365,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6BCDECB-3201-4C98-AA8D-79812894A18B}" name="Tabla19" displayName="Tabla19" ref="K34:N37" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6BCDECB-3201-4C98-AA8D-79812894A18B}" name="Tabla19" displayName="Tabla19" ref="K34:N37" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="K34:N37" xr:uid="{36798AE9-B843-4477-9F23-32045BDEF7D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E050CEA3-2793-4698-9E45-C3447ADCD555}" name="ID" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{03295AE7-34B5-4134-9D2F-2268D15B310C}" name="IDProducto" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{1564E106-D50F-4573-A696-EE197325F0F3}" name="IDAtributo" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{5F701778-C720-415C-9979-8380EB9AB80C}" name="Activo" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{E050CEA3-2793-4698-9E45-C3447ADCD555}" name="ID" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{03295AE7-34B5-4134-9D2F-2268D15B310C}" name="IDProducto" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{1564E106-D50F-4573-A696-EE197325F0F3}" name="IDAtributo" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{5F701778-C720-415C-9979-8380EB9AB80C}" name="Activo" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1281,8 +1384,8 @@
     <tableColumn id="1" xr3:uid="{76441B91-C9F3-418E-9F7A-2145EC66A51B}" name="ID"/>
     <tableColumn id="2" xr3:uid="{B7D7EADF-0604-4B90-A7CA-6537AE39152D}" name="Pronvincia"/>
     <tableColumn id="3" xr3:uid="{FBCCEEC7-DBEE-4480-8CBE-1F5805CA9202}" name="IdPais"/>
-    <tableColumn id="4" xr3:uid="{0A3D75EA-6C18-48E0-9489-C5D19B3AC70A}" name="Latitud" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{ACBD9873-D350-427F-993B-2B1B42296D9B}" name="Longitud" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{0A3D75EA-6C18-48E0-9489-C5D19B3AC70A}" name="Latitud" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{ACBD9873-D350-427F-993B-2B1B42296D9B}" name="Longitud" dataDxfId="34"/>
     <tableColumn id="6" xr3:uid="{957CA68C-6225-4C37-B8D5-8FF8C064FB1C}" name="Zoom"/>
     <tableColumn id="7" xr3:uid="{D19F9B22-3CC1-4E0E-B3DB-56D9B346F0CD}" name="Activo"/>
   </tableColumns>
@@ -1291,43 +1394,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D66B8F6B-A06F-42EB-B1CE-F5AC470DCC17}" name="Tabla20" displayName="Tabla20" ref="A62:D65" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A62:D65" xr:uid="{6995137C-E78D-4F26-A126-F3AEFE2A2B13}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7C1F763D-9A29-4F91-BB26-5F2CF68260F0}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{98E75056-4A9A-4C56-8FA5-EFD4D867777B}" name="Nombre" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{48A2AE2B-7A42-420C-8BB3-5F9F2AA01721}" name="Mail" dataDxfId="20">
-      <calculatedColumnFormula>CONCATENATE(B63,"@andez.com.ar")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D66B8F6B-A06F-42EB-B1CE-F5AC470DCC17}" name="Tabla20" displayName="Tabla20" ref="A62:E65" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A62:E65" xr:uid="{6995137C-E78D-4F26-A126-F3AEFE2A2B13}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7C1F763D-9A29-4F91-BB26-5F2CF68260F0}" name="ID" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F0BF2187-ECA7-4173-9FAC-3BC72EFDB82F}" name="IdEmpresa" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{98E75056-4A9A-4C56-8FA5-EFD4D867777B}" name="Nombre" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{48A2AE2B-7A42-420C-8BB3-5F9F2AA01721}" name="Mail" dataDxfId="21">
+      <calculatedColumnFormula>CONCATENATE(C63,"@andez.com.ar")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{31D99612-66DC-4B54-A747-6C39765D7B66}" name="Activo" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{31D99612-66DC-4B54-A747-6C39765D7B66}" name="Activo" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B2EAABA-4403-411A-98F0-A8284D43302C}" name="Tabla2021" displayName="Tabla2021" ref="F62:I65" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="F62:I65" xr:uid="{89087EED-CE2D-441A-9746-B0BA56EA9A63}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6D3F8F4E-2473-4BE6-A51E-C3C3E4C26133}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{12B007DF-889A-4CDB-93CC-EBEFCBD3A3E9}" name="Nombre" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{A94B5F86-8442-44DD-9C03-77F51D7F5B8D}" name="Telefono" dataDxfId="14">
-      <calculatedColumnFormula>CONCATENATE(G63,"@andez.com.ar")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B2EAABA-4403-411A-98F0-A8284D43302C}" name="Tabla2021" displayName="Tabla2021" ref="G62:K65" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="G62:K65" xr:uid="{89087EED-CE2D-441A-9746-B0BA56EA9A63}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6D3F8F4E-2473-4BE6-A51E-C3C3E4C26133}" name="ID" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{8C181956-53C7-4FD2-BAAB-42B1CDE2E84E}" name="IdEmpresa" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{12B007DF-889A-4CDB-93CC-EBEFCBD3A3E9}" name="Nombre" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{A94B5F86-8442-44DD-9C03-77F51D7F5B8D}" name="Telefono" dataDxfId="16">
+      <calculatedColumnFormula>CONCATENATE(I63,"@andez.com.ar")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0E412ADD-9FF3-43E1-BDA1-A917D6B1E4D7}" name="Activo" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0E412ADD-9FF3-43E1-BDA1-A917D6B1E4D7}" name="Activo" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{8F3FF2B6-156D-475C-B60E-2BBAE1F181CE}" name="Tabla21" displayName="Tabla21" ref="A69:D72" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A69:D72" xr:uid="{58000D4A-AEBA-4D49-B463-180C8FD8A937}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9F2D081-00F6-4B92-9DFE-6473CB6B3F38}" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{DE65DD1F-F1BA-4548-A19A-4B9DD2857A6F}" name="Red" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{23F951D4-E519-45F7-81C5-69ED4EA385E4}" name="URLRed" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{E5F1016C-C8F1-4FEA-B687-B57CB00F2E70}" name="Activo" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{8F3FF2B6-156D-475C-B60E-2BBAE1F181CE}" name="Tabla21" displayName="Tabla21" ref="A69:E72" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+  <autoFilter ref="A69:E72" xr:uid="{58000D4A-AEBA-4D49-B463-180C8FD8A937}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E9F2D081-00F6-4B92-9DFE-6473CB6B3F38}" name="ID" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{FE107DC5-A1C2-4F54-BC82-5BBB32CCABC3}" name="IdEmpresa" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{DE65DD1F-F1BA-4548-A19A-4B9DD2857A6F}" name="Red" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{23F951D4-E519-45F7-81C5-69ED4EA385E4}" name="URLRed" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{E5F1016C-C8F1-4FEA-B687-B57CB00F2E70}" name="Activo" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1347,12 +1453,18 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C769ADF8-2405-479D-8112-7564F0940768}" name="Tabla22" displayName="Tabla22" ref="F69:I72" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="F69:I72" xr:uid="{A2E83C68-75BA-4C98-B80E-E4E7E2B0B82C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{173EAAD2-F12F-4372-8FA2-00B32059C1EB}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{3E7AAA46-3847-4587-A43F-E688C1582045}" name="Titulo" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7727AE8E-759C-4DE1-86AE-BDFED86835D0}" name="Descripcion" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C769ADF8-2405-479D-8112-7564F0940768}" name="Tabla22" displayName="Tabla22" ref="A76:J77" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A76:J77" xr:uid="{A2E83C68-75BA-4C98-B80E-E4E7E2B0B82C}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{173EAAD2-F12F-4372-8FA2-00B32059C1EB}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3E7AAA46-3847-4587-A43F-E688C1582045}" name="RazonSocial" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7727AE8E-759C-4DE1-86AE-BDFED86835D0}" name="CUIT" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BBA783BB-BBBB-4233-929D-4BF68AFA091A}" name="Direccion" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{419A73DC-BE03-4D90-BE0C-9779F3EB2DDB}" name="Localidad" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{BE8C959F-F07F-4076-8E57-3EA25221B957}" name="Partido" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{DB60E2FA-C8A3-4C27-BCAB-41F7E5C99855}" name="IdProvincia" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{EC23197E-97BD-4D2B-AF77-BAEDEAEEEB33}" name="CP" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{7234FBEF-54AA-4FBE-8D11-84EDF024DAB3}" name="Horario" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{2D33166C-2999-4BC9-8B00-7F06B4D84FF1}" name="Activo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1395,7 +1507,7 @@
     <tableColumn id="4" xr3:uid="{33CF0639-7E0E-4323-ABAC-57E9E79BAC94}" name="URLManual"/>
     <tableColumn id="6" xr3:uid="{8FB3C041-5F4E-4C6B-BFEA-F7EF8CCA380F}" name="URLRepuestos"/>
     <tableColumn id="7" xr3:uid="{19883A37-D7EF-411E-B5D4-0F9C58EA4DF5}" name="URLPlanos"/>
-    <tableColumn id="5" xr3:uid="{9FBFC04D-E638-4A8E-BF60-60BF85B463B6}" name="Activo" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{9FBFC04D-E638-4A8E-BF60-60BF85B463B6}" name="Activo" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1422,7 +1534,7 @@
   <autoFilter ref="A6:G9" xr:uid="{00F67F5D-77F7-41B7-A265-5E336044A6C5}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F32EBD58-4145-475F-A8DD-60533C773560}" name="ID"/>
-    <tableColumn id="5" xr3:uid="{BA938A3C-223C-48BE-9D99-D519D9B88EDF}" name="Nombre" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{BA938A3C-223C-48BE-9D99-D519D9B88EDF}" name="Nombre" dataDxfId="53"/>
     <tableColumn id="2" xr3:uid="{BF58FE61-5919-4F9C-BC69-7F6F4B0BCCB1}" name="Apellido"/>
     <tableColumn id="4" xr3:uid="{B217BF12-7466-47C6-83EC-0600B0F7EE4B}" name="Mail">
       <calculatedColumnFormula>CONCATENATE(Tabla15[[#This Row],[Nombre]],Tabla15[[#This Row],[Apellido]],"@andez.com.ar")</calculatedColumnFormula>
@@ -1776,28 +1888,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD350C1D-1850-4BF9-ABCF-FA1A23EC1542}">
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:I33"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
@@ -2337,7 +2449,7 @@
         <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F27" t="s">
         <v>35</v>
@@ -2465,7 +2577,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="21"/>
       <c r="K33" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -3084,41 +3196,49 @@
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="22" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
-      <c r="F61" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="G61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
+      <c r="G61" s="22" t="s">
+        <v>137</v>
+      </c>
       <c r="H61" s="23"/>
-      <c r="I61" s="24"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="24"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="D62" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F62" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G62" s="10" t="s">
+      <c r="E62" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="I62" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="J62" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="I62" s="14" t="s">
+      <c r="K62" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3126,26 +3246,32 @@
       <c r="A63" s="13">
         <v>1</v>
       </c>
-      <c r="B63" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" s="10" t="str">
-        <f>CONCATENATE(B63,"@andez.com.ar")</f>
+      <c r="B63" s="25">
+        <v>1</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="25" t="str">
+        <f>CONCATENATE(C63,"@andez.com.ar")</f>
         <v>Compras@andez.com.ar</v>
       </c>
-      <c r="D63" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="13">
-        <v>1</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H63" s="10">
+      <c r="E63" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="13">
+        <v>1</v>
+      </c>
+      <c r="H63" s="25">
+        <v>1</v>
+      </c>
+      <c r="I63" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J63" s="25">
         <v>45552646</v>
       </c>
-      <c r="I63" s="14" t="b">
+      <c r="K63" s="14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3153,177 +3279,237 @@
       <c r="A64" s="13">
         <v>2</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="25">
+        <v>1</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" s="25" t="str">
+        <f t="shared" ref="D64:D65" si="0">CONCATENATE(C64,"@andez.com.ar")</f>
+        <v>RRHH@andez.com.ar</v>
+      </c>
+      <c r="E64" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="13">
+        <v>2</v>
+      </c>
+      <c r="H64" s="25">
+        <v>1</v>
+      </c>
+      <c r="I64" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J64" s="25">
+        <v>45552646</v>
+      </c>
+      <c r="K64" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="15">
+        <v>3</v>
+      </c>
+      <c r="B65" s="16">
+        <v>1</v>
+      </c>
+      <c r="C65" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="10" t="str">
-        <f t="shared" ref="C64:C65" si="0">CONCATENATE(B64,"@andez.com.ar")</f>
-        <v>RRHH@andez.com.ar</v>
-      </c>
-      <c r="D64" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="13">
-        <v>2</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H64" s="10">
-        <v>45552646</v>
-      </c>
-      <c r="I64" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="15">
-        <v>3</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="16" t="str">
+      <c r="D65" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Ventas@andez.com.ar</v>
       </c>
-      <c r="D65" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="15">
-        <v>3</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>130</v>
+      <c r="E65" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="15">
+        <v>3</v>
       </c>
       <c r="H65" s="16">
+        <v>1</v>
+      </c>
+      <c r="I65" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J65" s="16">
         <v>1545552646</v>
       </c>
-      <c r="I65" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K65" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="22" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
-      <c r="D68" s="24"/>
-      <c r="F68" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="24"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D68" s="23"/>
+      <c r="E68" s="24"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="13">
+        <v>1</v>
+      </c>
+      <c r="B70" s="25">
+        <v>1</v>
+      </c>
+      <c r="C70" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F69" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I69" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="13">
-        <v>1</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C70" s="10" t="s">
+      <c r="D70" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D70" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="13">
-        <v>1</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H70" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I70" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E70" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="13">
         <v>2</v>
       </c>
-      <c r="B71" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C71" s="10" t="s">
+      <c r="B71" s="25">
+        <v>1</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D71" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="13">
+      <c r="E71" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="15">
+        <v>3</v>
+      </c>
+      <c r="B72" s="16">
+        <v>1</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="24"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G76" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="J76" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="15">
+        <v>1</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G77" s="16">
         <v>2</v>
       </c>
-      <c r="G71" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="H71" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I71" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="15">
-        <v>3</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="15">
-        <v>3</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I72" s="17" t="b">
+      <c r="H77" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I77" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J77" s="17" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="F47:L47"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="G61:K61"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A75:J75"/>
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A12:E12"/>
@@ -3334,16 +3520,6 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="F19:L19"/>
     <mergeCell ref="K33:N33"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F47:L47"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>